<commit_message>
Minor updates Added Spotify Toybox library
</commit_message>
<xml_diff>
--- a/venv/static/Cubes/Test.xlsx
+++ b/venv/static/Cubes/Test.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Cube Info" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Cards" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -434,56 +434,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>cube_name</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>cube_description</t>
+          <t>card_name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>cube_is_cmdr</t>
+          <t>card_cid</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>cube_strats</t>
+          <t>card_strats</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>cube_pwd</t>
+          <t>card_tags</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Test test test</t>
+          <t>Ornithopter</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>UR</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>lorem, ipsum</t>
+          <t>Arf, Meow</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>Commander</t>
         </is>
       </c>
     </row>

</xml_diff>